<commit_message>
yaml olarak veri tabanı çıktısı alamama fix
</commit_message>
<xml_diff>
--- a/excels/fabrics.xlsx
+++ b/excels/fabrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,24 +470,128 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2024-06-02</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>300</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-02-06</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CD-2</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-02-22</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Test</t>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>cm2</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>200</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>cm2</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>200</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>

</xml_diff>